<commit_message>
Lecture 5 and story on project 1
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE7DC6AC-E7EE-42BC-AC3E-264D895EA9E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82734889-2FF9-41D9-BBDC-787F1371A88F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
@@ -606,16 +606,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>162606</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>360161</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28222</xdr:rowOff>
+      <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>261408</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>458963</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>55739</xdr:rowOff>
+      <xdr:rowOff>196851</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,7 +645,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5538939" y="28222"/>
+          <a:off x="6279772" y="169334"/>
           <a:ext cx="2525913" cy="2242961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -668,15 +668,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>398406</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>98778</xdr:rowOff>
+      <xdr:colOff>102073</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>546101</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>17638</xdr:rowOff>
+      <xdr:colOff>249768</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>208138</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -706,7 +706,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8201850" y="282222"/>
+          <a:off x="9055573" y="28222"/>
           <a:ext cx="5001917" cy="3390194"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -728,16 +728,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>303388</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>451554</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>162278</xdr:rowOff>
+      <xdr:rowOff>119944</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>449438</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>597604</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>115712</xdr:rowOff>
+      <xdr:rowOff>73378</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -767,7 +767,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6829777" y="2596445"/>
+          <a:off x="6371165" y="2554111"/>
           <a:ext cx="3786717" cy="2486378"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Project 1 description, excel data
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82734889-2FF9-41D9-BBDC-787F1371A88F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F739E39-1D2E-4332-BF99-52333DDF52EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Water-Delivery" sheetId="1" r:id="rId1"/>
+    <sheet name="Hospital-Distribution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t>Pipe</t>
   </si>
@@ -345,21 +346,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>13</t>
-    </r>
-  </si>
-  <si>
     <t>Diameter</t>
   </si>
   <si>
@@ -367,22 +353,6 @@
   </si>
   <si>
     <t>cm</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Duct Dimensions </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>h,w</t>
-    </r>
   </si>
   <si>
     <t>Height [in]</t>
@@ -407,6 +377,390 @@
       </rPr>
       <t xml:space="preserve">h </t>
     </r>
+  </si>
+  <si>
+    <t>Pipe Dimensions L</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Length L</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Water Per Hospital Bed</t>
+  </si>
+  <si>
+    <t>gal/day</t>
+  </si>
+  <si>
+    <t>OHSU Bed Count</t>
+  </si>
+  <si>
+    <t>beds</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Non-Circular Dimensions </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>h,w</t>
+    </r>
+  </si>
+  <si>
+    <t>Price of Energy</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>Pipe System Components</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Union Threaded</t>
+  </si>
+  <si>
+    <t>Line Flow Flanged</t>
+  </si>
+  <si>
+    <t>Line Flow Threaded</t>
+  </si>
+  <si>
+    <t>Swing Check Forward Flow</t>
+  </si>
+  <si>
+    <t>Branch Flow, Flanged</t>
+  </si>
+  <si>
+    <t>Ball Valve Fully Open</t>
+  </si>
+  <si>
+    <t>Gate Fully Open</t>
+  </si>
+  <si>
+    <t>Gate 1/4 Closed</t>
+  </si>
+  <si>
+    <t>Pipe Expansion/Contractions</t>
+  </si>
+  <si>
+    <t>1-&gt;2</t>
+  </si>
+  <si>
+    <t>2-&gt;3</t>
+  </si>
+  <si>
+    <t>3-&gt;4</t>
+  </si>
+  <si>
+    <t>4-&gt;5</t>
+  </si>
+  <si>
+    <t>5-&gt;6</t>
+  </si>
+  <si>
+    <t>6-&gt;7</t>
+  </si>
+  <si>
+    <t>7-&gt;8</t>
+  </si>
+  <si>
+    <t>8-&gt;9</t>
+  </si>
+  <si>
+    <t>9-&gt;10</t>
+  </si>
+  <si>
+    <t>10-&gt;11</t>
+  </si>
+  <si>
+    <t>11-&gt;12</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tot</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tot</t>
+    </r>
+  </si>
+  <si>
+    <t>Friction Factor</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -416,7 +770,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,6 +858,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -519,7 +905,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -558,31 +944,349 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -606,16 +1310,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>360161</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>564772</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>458963</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>196851</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>56796</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>6349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -645,7 +1349,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6279772" y="169334"/>
+          <a:off x="10125050" y="388055"/>
           <a:ext cx="2525913" cy="2242961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -668,15 +1372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>102073</xdr:colOff>
+      <xdr:colOff>333495</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28222</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>249768</xdr:colOff>
+      <xdr:colOff>484012</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>208138</xdr:rowOff>
+      <xdr:rowOff>164394</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -706,8 +1410,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9055573" y="28222"/>
-          <a:ext cx="5001917" cy="3390194"/>
+          <a:off x="10341095" y="0"/>
+          <a:ext cx="5027317" cy="3424061"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -729,15 +1433,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>451554</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>119944</xdr:rowOff>
+      <xdr:colOff>330198</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>597604</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>73378</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>289981</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>39511</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -767,8 +1471,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6371165" y="2554111"/>
-          <a:ext cx="3786717" cy="2486378"/>
+          <a:off x="6265331" y="0"/>
+          <a:ext cx="3803650" cy="2511778"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -790,15 +1494,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>472722</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>218719</xdr:rowOff>
+      <xdr:colOff>328790</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>593373</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>139698</xdr:rowOff>
+      <xdr:colOff>449440</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -828,8 +1532,252 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10033000" y="3654775"/>
-          <a:ext cx="3761317" cy="1233312"/>
+          <a:off x="11326990" y="142520"/>
+          <a:ext cx="3778250" cy="1241779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>475478</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1174043</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>11286</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C000A956-E223-43FB-B0CF-69BFC5BCE1DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3430345" y="6417734"/>
+          <a:ext cx="2239498" cy="2898419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>148973</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>181328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B45E53-CD83-4BE9-8BFF-BE01FEA1EF7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2494240" y="9745134"/>
+          <a:ext cx="2515910" cy="2357260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>320321</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>40920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>440971</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>131232</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B880DA8-DE91-4618-AD65-D16491812DA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11318521" y="1361720"/>
+          <a:ext cx="3778250" cy="1241779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>118532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>471056</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114297</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BC8C23-0A87-4E63-BFCD-B6AE9F3E8766}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11150600" y="4919132"/>
+          <a:ext cx="3976256" cy="2823632"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1148,10 +2096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,17 +2109,25 @@
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="10.54296875" customWidth="1"/>
     <col min="7" max="7" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="F1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,8 +2140,14 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="34">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1196,11 +2158,11 @@
       <c r="C3" s="2">
         <v>9</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>2.35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1210,12 +2172,16 @@
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1.1299999999999999</v>
       </c>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1225,11 +2191,17 @@
       <c r="C5" s="2">
         <v>0.9</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F5" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="34">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1239,11 +2211,11 @@
       <c r="C6" s="2">
         <v>0.26</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>2.34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1253,11 +2225,15 @@
       <c r="C7" s="2">
         <v>0.15</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>3.21</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1267,11 +2243,17 @@
       <c r="C8" s="2">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="37">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1281,11 +2263,11 @@
       <c r="C9" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>4.1500000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1295,135 +2277,694 @@
       <c r="C10" s="2">
         <v>0</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="7" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
+    <row r="14" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="11" t="s">
+      <c r="K17" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="L17" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
         <v>36</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2">
+        <v>340</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18" s="2">
+        <v>12</v>
+      </c>
+      <c r="J18" s="2">
+        <v>36</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A19" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>36</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="10" t="s">
+      <c r="E19" s="2">
+        <v>4321</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="27"/>
+      <c r="I19" s="2">
+        <v>24</v>
+      </c>
+      <c r="J19" s="2">
+        <v>36</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="12">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>36</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1456</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="2">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2">
+        <v>48</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A21" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="48">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="48">
+        <v>2655</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="14">
+        <v>12</v>
+      </c>
+      <c r="J21" s="14">
+        <v>48</v>
+      </c>
+      <c r="K21" s="14"/>
+      <c r="L21" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="48">
+        <v>24</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="48">
+        <v>7655</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="K22" t="s">
+        <v>86</v>
+      </c>
+      <c r="L22">
+        <f>SUM(L18:L21)</f>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A23" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="48">
+        <v>36</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="48">
+        <v>1221</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A24" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="48">
+        <v>36</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="48">
+        <v>900</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A25" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="48">
+        <v>48</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="48">
+        <v>765</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A26" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="48">
+        <v>48</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="48">
+        <v>250</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="48">
+        <v>24</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="48">
+        <v>550</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="27"/>
+    </row>
+    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="48">
+        <v>24</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="48">
+        <v>457</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="27"/>
+    </row>
+    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="A29" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="14">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A19" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A20" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A22" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A23" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A24" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A25" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A26" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A27" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A28" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A29" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.45">
-      <c r="A30" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="14">
+        <v>788</v>
+      </c>
+      <c r="F29" s="15"/>
+      <c r="G29" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="28"/>
+    </row>
+    <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.45">
+      <c r="D30" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30">
+        <f>SUM(E18:E29) + L22</f>
+        <v>21808</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="44"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="54"/>
+      <c r="C32" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="12"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="12"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="12"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="12"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="12"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="12"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="12"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="12"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="12"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="12"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="11">
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="D16:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C807-0474-4350-8CC5-BCF0B4090853}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project 1 complete, project 1 grading rubric
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F739E39-1D2E-4332-BF99-52333DDF52EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524EAA75-D00D-4ABF-AF2D-247D601A37F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Water-Delivery" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
   <si>
     <t>Pipe</t>
   </si>
@@ -762,6 +762,76 @@
   <si>
     <t>f</t>
   </si>
+  <si>
+    <t>Diameter [in]</t>
+  </si>
+  <si>
+    <t>Length [ft]</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pipe </t>
+  </si>
+  <si>
+    <t>Ball Valve (Open)</t>
+  </si>
+  <si>
+    <t>Branch Flow (T)</t>
+  </si>
+  <si>
+    <t>Level 1 Pipe Dimensions and Components: z=0</t>
+  </si>
+  <si>
+    <t>Qmin</t>
+  </si>
+  <si>
+    <t>Qmax</t>
+  </si>
+  <si>
+    <t>Level 1:  Flow Rate [gal/min]</t>
+  </si>
+  <si>
+    <t>Level 2:  Flow Rate [gal/min]</t>
+  </si>
+  <si>
+    <t>Level 3:  Flow Rate [gal/min]</t>
+  </si>
+  <si>
+    <t>Old Cast Iron</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">All Piping Material </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mm]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 2 Pipe Dimensions and Components: z=15ft, D = 8 in </t>
+  </si>
+  <si>
+    <t>Level 3 Pipe Dimensions and Components: z = 30ft, D = 8in</t>
+  </si>
 </sst>
 </file>
 
@@ -770,7 +840,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +959,16 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1195,7 +1275,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1203,32 +1283,11 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1261,16 +1320,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1287,6 +1337,51 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1555,15 +1650,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>475478</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>110067</xdr:rowOff>
+      <xdr:colOff>77545</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>107091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1174043</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>11286</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>550333</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>129820</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1593,8 +1688,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3430345" y="6417734"/>
-          <a:ext cx="2239498" cy="2898419"/>
+          <a:off x="3032412" y="2960358"/>
+          <a:ext cx="5146388" cy="6660595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1794,6 +1889,2178 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>493889</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>237058</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93161</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AD439CD-980D-4690-8516-1015F9E6D065}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6618111" y="3971894"/>
+          <a:ext cx="1979780" cy="157045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74580</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>30846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>358963</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>4446</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26D28008-A349-4421-AE02-DF52012B0909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="8435413" y="2232179"/>
+          <a:ext cx="3318272" cy="157045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74581</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>141115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>237058</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93159</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34540C7-8FC8-4580-92A0-F3135F1287E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="6614464" y="2145509"/>
+          <a:ext cx="3804378" cy="162477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74581</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>119559</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>234027</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>93159</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2EA760C-88A8-4841-93E0-B5BFC5D2E094}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8435414" y="3971892"/>
+          <a:ext cx="1979780" cy="157045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74578</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>141112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>360890</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114712</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AEA1859-A4F9-4A34-AFED-96D0AC3CFB43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="8435411" y="324556"/>
+          <a:ext cx="4533757" cy="157045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>760051</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>134702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370032</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>137145</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Isosceles Triangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{900730E5-3F1E-486F-A5A7-5B6F4C46AA2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8302440" y="1051924"/>
+          <a:ext cx="428425" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>760051</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370032</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>54499</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Isosceles Triangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCB846E-28E8-455A-91CC-A5CB599867F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8302440" y="2987167"/>
+          <a:ext cx="428425" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>421815</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80371</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50193</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>82814</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CD22DC8-3B5C-4BC0-848B-9CE83396770B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8782648" y="3015482"/>
+          <a:ext cx="2662267" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Ball Valves, Open, D = 8 in </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>370032</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>12730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>605188</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>15173</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39B6007-F99A-4C79-8B66-45B0B53F2A95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8730865" y="1113397"/>
+          <a:ext cx="2662267" cy="369332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Ball Valves, Open, D = 8 in </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>83351</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>172063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>462492</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>20276</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Arrow: Down 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F04917E-CE5E-4F2E-9C19-FFB0B756CB49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11478073" y="2006507"/>
+          <a:ext cx="379141" cy="765436"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>570737</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>29622</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>343100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Arrow: Down 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D6BB91-3E3F-4AAD-9012-E40C41B66817}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10145126" y="3698511"/>
+          <a:ext cx="379141" cy="765436"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>80529</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>70464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>459670</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102122</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Arrow: Down 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7176E8F5-2B62-4846-8329-3FDFB492D73D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12688807" y="70464"/>
+          <a:ext cx="379141" cy="765436"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>24085</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>14020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>183529</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>165189</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="18" name="Group 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B796823D-9966-4C15-95FF-4CA6FC65984C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6148307" y="3499464"/>
+          <a:ext cx="1577611" cy="1435281"/>
+          <a:chOff x="3264529" y="4477194"/>
+          <a:chExt cx="1638753" cy="1490907"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Isosceles Triangle 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{745FB8B8-6E2C-49B5-BBB9-8780F47809B9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3264529" y="4555383"/>
+            <a:ext cx="1638753" cy="1412718"/>
+          </a:xfrm>
+          <a:prstGeom prst="triangle">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="en-US"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Oval 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711B5C3F-93D2-4A59-B46D-9F2173F658DC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3472247" y="4477194"/>
+            <a:ext cx="1223319" cy="1223319"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="en-US"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pump</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2098,8 +4365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A18" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2116,16 +4383,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="F1" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -2140,10 +4407,10 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="34">
+      <c r="G2" s="27">
         <v>345</v>
       </c>
     </row>
@@ -2176,10 +4443,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -2194,10 +4461,10 @@
       <c r="D5" s="4">
         <v>0.65</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="27">
         <v>522</v>
       </c>
     </row>
@@ -2228,10 +4495,10 @@
       <c r="D7" s="4">
         <v>3.21</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -2246,10 +4513,10 @@
       <c r="D8" s="5">
         <v>2.13</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="30">
         <v>13.12</v>
       </c>
     </row>
@@ -2282,109 +4549,109 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
     </row>
     <row r="13" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="8" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="26" t="s">
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="10"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="47"/>
     </row>
     <row r="17" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K17" s="24" t="s">
+      <c r="K17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>36</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="21" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="2">
         <v>340</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="39" t="s">
+      <c r="F18" s="8"/>
+      <c r="G18" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="27"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="2">
         <v>12</v>
       </c>
@@ -2392,29 +4659,29 @@
         <v>36</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="12">
+      <c r="L18" s="8">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>36</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="21" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="2">
         <v>4321</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="38" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="27"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="2">
         <v>24</v>
       </c>
@@ -2422,29 +4689,29 @@
         <v>36</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="12">
+      <c r="L19" s="8">
         <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="2">
         <v>36</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="21" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="2">
         <v>1456</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="39" t="s">
+      <c r="F20" s="8"/>
+      <c r="G20" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="27"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="2">
         <v>12</v>
       </c>
@@ -2452,59 +4719,59 @@
         <v>48</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="12">
+      <c r="L20" s="8">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="38">
         <v>24</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="21" t="s">
+      <c r="C21" s="8"/>
+      <c r="D21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="38">
         <v>2655</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="39" t="s">
+      <c r="F21" s="8"/>
+      <c r="G21" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="14">
+      <c r="H21" s="20"/>
+      <c r="I21" s="10">
         <v>12</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="10">
         <v>48</v>
       </c>
-      <c r="K21" s="14"/>
-      <c r="L21" s="15">
+      <c r="K21" s="10"/>
+      <c r="L21" s="11">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="38">
         <v>24</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="21" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="38">
         <v>7655</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="39" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="27"/>
+      <c r="H22" s="20"/>
       <c r="K22" t="s">
         <v>86</v>
       </c>
@@ -2514,147 +4781,147 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="48">
+      <c r="B23" s="38">
         <v>36</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="21" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="48">
+      <c r="E23" s="38">
         <v>1221</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="38" t="s">
+      <c r="F23" s="8"/>
+      <c r="G23" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="27"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="38">
         <v>36</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="21" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="38">
         <v>900</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="38" t="s">
+      <c r="F24" s="8"/>
+      <c r="G24" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="27"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="48">
+      <c r="B25" s="38">
         <v>48</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="21" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="38">
         <v>765</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="38" t="s">
+      <c r="F25" s="8"/>
+      <c r="G25" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="48">
+      <c r="B26" s="38">
         <v>48</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="21" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="48">
+      <c r="E26" s="38">
         <v>250</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="39" t="s">
+      <c r="F26" s="8"/>
+      <c r="G26" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="27"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="48">
+      <c r="B27" s="38">
         <v>24</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="21" t="s">
+      <c r="C27" s="8"/>
+      <c r="D27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="38">
         <v>550</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="39" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="27"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="38">
         <v>24</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="21" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="48">
+      <c r="E28" s="38">
         <v>457</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="39" t="s">
+      <c r="F28" s="8"/>
+      <c r="G28" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="27"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="10">
         <v>18</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="22" t="s">
+      <c r="C29" s="11"/>
+      <c r="D29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="10">
         <v>788</v>
       </c>
-      <c r="F29" s="15"/>
-      <c r="G29" s="40" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="28"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="1:12" ht="17" x14ac:dyDescent="0.45">
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="39" t="s">
         <v>87</v>
       </c>
       <c r="E30">
@@ -2663,279 +4930,279 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="44"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="44"/>
+      <c r="C32" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="42" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="12">
+      <c r="C33" s="36"/>
+      <c r="D33" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="12">
+      <c r="C34" s="20"/>
+      <c r="D34" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="12">
+      <c r="C35" s="20"/>
+      <c r="D35" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="12">
+      <c r="C36" s="20"/>
+      <c r="D36" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="12">
+      <c r="C37" s="20"/>
+      <c r="D37" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="12">
+      <c r="C38" s="20"/>
+      <c r="D38" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="12">
+      <c r="C39" s="20"/>
+      <c r="D39" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="12">
+      <c r="C40" s="20"/>
+      <c r="D40" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="12">
+      <c r="C41" s="20"/>
+      <c r="D41" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="12">
+      <c r="C42" s="20"/>
+      <c r="D42" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="12">
+      <c r="C43" s="20"/>
+      <c r="D43" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="12">
+      <c r="C44" s="20"/>
+      <c r="D44" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="12">
+      <c r="C45" s="20"/>
+      <c r="D45" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B46" s="2"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="12">
+      <c r="C46" s="20"/>
+      <c r="D46" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="2"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="12">
+      <c r="C47" s="20"/>
+      <c r="D47" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="15">
+      <c r="B48" s="10"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="10"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="47"/>
     </row>
     <row r="51" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="35" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="12"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="12"/>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="2"/>
-      <c r="C54" s="12"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B55" s="2"/>
-      <c r="C55" s="12"/>
+      <c r="C55" s="8"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="12"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="12"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="12"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="12"/>
+      <c r="C59" s="8"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="12"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="12"/>
+      <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2959,12 +5226,455 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C807-0474-4350-8CC5-BCF0B4090853}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
+      <c r="G1" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="62"/>
+      <c r="J1" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="57"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="8"/>
+      <c r="G3" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="11">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10">
+        <v>10</v>
+      </c>
+      <c r="C9" s="10">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
+      <c r="G10" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="H10" s="62"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="8"/>
+      <c r="G12" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="11">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="7">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
+        <v>7</v>
+      </c>
+      <c r="B18" s="10">
+        <v>10</v>
+      </c>
+      <c r="C18" s="10">
+        <v>8</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="G19" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="62"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="8"/>
+      <c r="G21" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="11">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="7">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="7">
+        <v>6</v>
+      </c>
+      <c r="B26" s="2">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="9">
+        <v>7</v>
+      </c>
+      <c r="B27" s="10">
+        <v>10</v>
+      </c>
+      <c r="C27" s="10">
+        <v>8</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
connors code + project excel unit fix
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA6466C-254D-4728-B256-F366ED3C814E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F683AC-3D94-4FA0-BCB9-FBBC7468BEEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Water-Delivery" sheetId="1" r:id="rId1"/>
@@ -565,9 +565,6 @@
     <t>Length</t>
   </si>
   <si>
-    <t>Length L</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -778,9 +775,6 @@
     <t>Ball Valve (Open)</t>
   </si>
   <si>
-    <t>Branch Flow (T)</t>
-  </si>
-  <si>
     <t>Level 1 Pipe Dimensions and Components: z=0</t>
   </si>
   <si>
@@ -831,6 +825,25 @@
   </si>
   <si>
     <t>Level 3 Pipe Dimensions and Components: z = 30ft, D = 8in</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Length L </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[ft]</t>
+    </r>
+  </si>
+  <si>
+    <t>Branch Flow (Threaded)</t>
   </si>
 </sst>
 </file>
@@ -1334,6 +1347,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1379,10 +1396,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4366,8 +4379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView topLeftCell="A30" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4381,19 +4394,20 @@
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="F1" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="50"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="F1" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -4409,7 +4423,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" s="24">
         <v>345</v>
@@ -4444,10 +4458,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="50"/>
+      <c r="F4" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="54"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -4463,7 +4477,7 @@
         <v>0.65</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="24">
         <v>522</v>
@@ -4496,10 +4510,10 @@
       <c r="D7" s="4">
         <v>3.21</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="50"/>
+      <c r="F7" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="54"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -4515,7 +4529,7 @@
         <v>2.13</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="27">
         <v>13.12</v>
@@ -4550,11 +4564,11 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
     </row>
     <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
@@ -4573,29 +4587,29 @@
       <c r="C14" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="54"/>
       <c r="G16" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="I16" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="50"/>
+        <v>87</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="54"/>
     </row>
     <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="20" t="s">
@@ -4614,28 +4628,28 @@
         <v>2</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="62" t="s">
+      <c r="J17" s="47" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
@@ -4667,7 +4681,7 @@
       <c r="L18" s="8">
         <v>25</v>
       </c>
-      <c r="M18" s="63" t="s">
+      <c r="M18" s="48" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4700,7 +4714,7 @@
       <c r="L19" s="8">
         <v>125</v>
       </c>
-      <c r="M19" s="63" t="s">
+      <c r="M19" s="48" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4733,7 +4747,7 @@
       <c r="L20" s="8">
         <v>200</v>
       </c>
-      <c r="M20" s="63" t="s">
+      <c r="M20" s="48" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4766,7 +4780,7 @@
       <c r="L21" s="11">
         <v>100</v>
       </c>
-      <c r="M21" s="64" t="s">
+      <c r="M21" s="49" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4790,7 +4804,7 @@
       </c>
       <c r="H22" s="17"/>
       <c r="K22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L22">
         <f>SUM(L18:L21)</f>
@@ -4939,7 +4953,7 @@
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.45">
       <c r="D30" s="36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E30">
         <f>SUM(E18:E29) + L22</f>
@@ -4947,20 +4961,20 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="53"/>
-    </row>
-    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="46" t="s">
+      <c r="B32" s="51"/>
+      <c r="C32" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="D32" s="39" t="s">
         <v>0</v>
@@ -4968,7 +4982,7 @@
     </row>
     <row r="33" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="33"/>
@@ -4978,7 +4992,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="17"/>
@@ -4988,7 +5002,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="17"/>
@@ -4998,7 +5012,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="17"/>
@@ -5008,7 +5022,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="17"/>
@@ -5018,7 +5032,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="17"/>
@@ -5028,7 +5042,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="17"/>
@@ -5038,7 +5052,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="17"/>
@@ -5048,7 +5062,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="17"/>
@@ -5058,7 +5072,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="17"/>
@@ -5068,7 +5082,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="17"/>
@@ -5078,7 +5092,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="17"/>
@@ -5088,7 +5102,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="17"/>
@@ -5098,7 +5112,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="17"/>
@@ -5108,7 +5122,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="17"/>
@@ -5118,7 +5132,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="18"/>
@@ -5127,102 +5141,103 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B50" s="49"/>
-      <c r="C50" s="50"/>
+      <c r="A50" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="53"/>
+      <c r="C50" s="54"/>
     </row>
     <row r="51" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>85</v>
-      </c>
       <c r="C51" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="8"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="8"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I16:M16"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A50:C50"/>
     <mergeCell ref="A31:D31"/>
@@ -5233,7 +5248,6 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="I16:M16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5245,8 +5259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C807-0474-4350-8CC5-BCF0B4090853}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5263,46 +5277,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="A1" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
       <c r="G1" s="43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" s="44"/>
-      <c r="J1" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="60"/>
+      <c r="J1" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="64"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>92</v>
-      </c>
       <c r="E2" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2" s="8">
         <v>1.5</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K2" s="11">
         <v>0.28000000000000003</v>
@@ -5321,7 +5335,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="8"/>
       <c r="G3" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" s="11">
         <v>6.5</v>
@@ -5351,7 +5365,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="8"/>
     </row>
@@ -5379,7 +5393,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E7" s="8"/>
     </row>
@@ -5410,36 +5424,36 @@
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="60"/>
+      <c r="A10" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
       <c r="G10" s="43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>92</v>
-      </c>
       <c r="E11" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H11" s="8">
         <v>1.5</v>
@@ -5458,7 +5472,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="8"/>
       <c r="G12" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H12" s="11">
         <v>4.5</v>
@@ -5488,7 +5502,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="8"/>
     </row>
@@ -5516,7 +5530,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E16" s="8"/>
     </row>
@@ -5547,36 +5561,36 @@
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
       <c r="G19" s="43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H19" s="44"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" s="41" t="s">
-        <v>92</v>
-      </c>
       <c r="E20" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" s="45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" s="8">
         <v>1.5</v>
@@ -5595,7 +5609,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="8"/>
       <c r="G21" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H21" s="11">
         <v>3.6</v>
@@ -5625,7 +5639,7 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -5653,7 +5667,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E25" s="8"/>
     </row>

</xml_diff>

<commit_message>
Project 2 finalized w/ new due date!
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20357"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20358"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F683AC-3D94-4FA0-BCB9-FBBC7468BEEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32FBAD7-30A9-451C-A16C-6D95A59E0B18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
@@ -1351,12 +1351,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1364,6 +1358,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4404,10 +4404,10 @@
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
       <c r="D1" s="58"/>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="54"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -4458,10 +4458,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="52"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -4510,10 +4510,10 @@
       <c r="D7" s="4">
         <v>3.21</v>
       </c>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="54"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -4587,29 +4587,29 @@
       <c r="C14" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="52" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="54"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H16" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="54"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="52"/>
     </row>
     <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="20" t="s">
@@ -4969,10 +4969,10 @@
       <c r="D31" s="57"/>
     </row>
     <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="50" t="s">
+      <c r="A32" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="51"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="13" t="s">
         <v>62</v>
       </c>
@@ -5141,11 +5141,11 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="52" t="s">
+      <c r="A50" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="53"/>
-      <c r="C50" s="54"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="52"/>
     </row>
     <row r="51" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A51" s="34" t="s">

</xml_diff>

<commit_message>
Final posted, I'm so sorry, so sorry.
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32FBAD7-30A9-451C-A16C-6D95A59E0B18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E759CFCC-8950-43AB-A1C1-4A1735B54D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
@@ -1663,14 +1663,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>568612</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>610946</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>30891</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>524934</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1210734</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>62086</xdr:rowOff>
     </xdr:to>
@@ -1702,7 +1702,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2304279" y="4611358"/>
+          <a:off x="4370146" y="4611358"/>
           <a:ext cx="5146388" cy="6660595"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3787,7 +3787,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6148307" y="3499464"/>
+          <a:off x="6733918" y="3499464"/>
           <a:ext cx="1577611" cy="1435281"/>
           <a:chOff x="3264529" y="4477194"/>
           <a:chExt cx="1638753" cy="1490907"/>
@@ -4379,7 +4379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -5260,7 +5260,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5268,7 +5268,7 @@
     <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" customWidth="1"/>
     <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="11.26953125" customWidth="1"/>

</xml_diff>

<commit_message>
project ppt typo fixed
</commit_message>
<xml_diff>
--- a/projects/Project-1-Data.xlsx
+++ b/projects/Project-1-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205D40C4-E05C-4EAD-A52A-14A1A6C34DFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B50E2-D37A-462B-8643-E7EE4F20BA6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{93FF287D-E21B-45B2-BB89-59A7DA375D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Water-Delivery" sheetId="1" r:id="rId1"/>
@@ -2207,7 +2207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E90A3597-DF8E-467A-A322-23FDFFEE6126}">
   <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -3087,7 +3087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F2C807-0474-4350-8CC5-BCF0B4090853}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>